<commit_message>
Test and document switches etc.
</commit_message>
<xml_diff>
--- a/tests/test1/output/main-loc.xlsx
+++ b/tests/test1/output/main-loc.xlsx
@@ -506,6 +506,78 @@
   </x:si>
   <x:si>
     <x:t>And we're back.</x:t>
+  </x:si>
+  <x:si>
+    <x:t>cycles_Cycles_LineTest_65J9</x:t>
+  </x:si>
+  <x:si>
+    <x:t>This should be fine.</x:t>
+  </x:si>
+  <x:si>
+    <x:t>cycles_Cycles_LineTest_XFQW</x:t>
+  </x:si>
+  <x:si>
+    <x:t>So should this.</x:t>
+  </x:si>
+  <x:si>
+    <x:t>cycles_Cycles_FancyBarkTest_RR4G</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Fancy Bark 1</x:t>
+  </x:si>
+  <x:si>
+    <x:t>cycles_Cycles_FancyBarkTest_D4KV</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Fancy Bark 2</x:t>
+  </x:si>
+  <x:si>
+    <x:t>cycles_Cycles_FancyBarkTest_A2I1</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Fancy Bark 3</x:t>
+  </x:si>
+  <x:si>
+    <x:t>cycles_Cycles_FancyBarkTest_3KK1</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Fancy Bark 4</x:t>
+  </x:si>
+  <x:si>
+    <x:t>cycles_Cycles_FancyBarkTest_FF35</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Spinning on fancy bark 5</x:t>
+  </x:si>
+  <x:si>
+    <x:t>cycles_Cycles_FancyBarkTest_23Q8</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Spinning on fancy bark 6</x:t>
+  </x:si>
+  <x:si>
+    <x:t>cycles_Cycles_StringExpressionsTest_1L9A</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Huh.</x:t>
+  </x:si>
+  <x:si>
+    <x:t>cycles_Cycles_StringExpressionsTest_ZHNZ</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Huh yourself.</x:t>
+  </x:si>
+  <x:si>
+    <x:t>cycles_Cycles_ListExpressionTest_LUCG</x:t>
+  </x:si>
+  <x:si>
+    <x:t>List item 1.</x:t>
+  </x:si>
+  <x:si>
+    <x:t>cycles_Cycles_ListExpressionTest_JXXD</x:t>
+  </x:si>
+  <x:si>
+    <x:t>List item 2.</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -596,8 +668,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<x:table xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:D78" totalsRowShown="0">
-  <x:autoFilter ref="A1:D78"/>
+<x:table xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:D90" totalsRowShown="0">
+  <x:autoFilter ref="A1:D90"/>
   <x:tableColumns count="4">
     <x:tableColumn id="1" name="ID" dataDxfId="0"/>
     <x:tableColumn id="2" name="Text" dataDxfId="0"/>
@@ -896,7 +968,7 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:D78"/>
+  <x:dimension ref="A1:D90"/>
   <x:sheetViews>
     <x:sheetView workbookViewId="0">
       <x:pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
@@ -905,7 +977,7 @@
   <x:sheetFormatPr defaultRowHeight="15"/>
   <x:cols>
     <x:col min="5" max="16384" width="9.140625" style="1" customWidth="1"/>
-    <x:col min="1" max="1" width="34.585625" style="1" customWidth="1"/>
+    <x:col min="1" max="1" width="39.210625" style="1" customWidth="1"/>
     <x:col min="2" max="2" width="37.960625" style="1" customWidth="1"/>
     <x:col min="3" max="3" width="9.960625" style="1" customWidth="1"/>
     <x:col min="4" max="4" width="48.210625" style="1" customWidth="1"/>
@@ -2000,6 +2072,174 @@
         <x:v>32</x:v>
       </x:c>
       <x:c r="D78" s="1" t="s">
+        <x:v>6</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="79" spans="1:4" ht="13.5" customHeight="1">
+      <x:c r="A79" s="1" t="s">
+        <x:v>164</x:v>
+      </x:c>
+      <x:c r="B79" s="1" t="s">
+        <x:v>165</x:v>
+      </x:c>
+      <x:c r="C79" s="1" t="s">
+        <x:v>18</x:v>
+      </x:c>
+      <x:c r="D79" s="1" t="s">
+        <x:v>6</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="80" spans="1:4" ht="13.5" customHeight="1">
+      <x:c r="A80" s="1" t="s">
+        <x:v>166</x:v>
+      </x:c>
+      <x:c r="B80" s="1" t="s">
+        <x:v>167</x:v>
+      </x:c>
+      <x:c r="C80" s="1" t="s">
+        <x:v>86</x:v>
+      </x:c>
+      <x:c r="D80" s="1" t="s">
+        <x:v>6</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="81" spans="1:4" ht="13.5" customHeight="1">
+      <x:c r="A81" s="1" t="s">
+        <x:v>168</x:v>
+      </x:c>
+      <x:c r="B81" s="1" t="s">
+        <x:v>169</x:v>
+      </x:c>
+      <x:c r="C81" s="1" t="s">
+        <x:v>18</x:v>
+      </x:c>
+      <x:c r="D81" s="1" t="s">
+        <x:v>6</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="82" spans="1:4" ht="13.5" customHeight="1">
+      <x:c r="A82" s="1" t="s">
+        <x:v>170</x:v>
+      </x:c>
+      <x:c r="B82" s="1" t="s">
+        <x:v>171</x:v>
+      </x:c>
+      <x:c r="C82" s="1" t="s">
+        <x:v>18</x:v>
+      </x:c>
+      <x:c r="D82" s="1" t="s">
+        <x:v>6</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="83" spans="1:4" ht="13.5" customHeight="1">
+      <x:c r="A83" s="1" t="s">
+        <x:v>172</x:v>
+      </x:c>
+      <x:c r="B83" s="1" t="s">
+        <x:v>173</x:v>
+      </x:c>
+      <x:c r="C83" s="1" t="s">
+        <x:v>18</x:v>
+      </x:c>
+      <x:c r="D83" s="1" t="s">
+        <x:v>6</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="84" spans="1:4" ht="13.5" customHeight="1">
+      <x:c r="A84" s="1" t="s">
+        <x:v>174</x:v>
+      </x:c>
+      <x:c r="B84" s="1" t="s">
+        <x:v>175</x:v>
+      </x:c>
+      <x:c r="C84" s="1" t="s">
+        <x:v>18</x:v>
+      </x:c>
+      <x:c r="D84" s="1" t="s">
+        <x:v>6</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="85" spans="1:4" ht="13.5" customHeight="1">
+      <x:c r="A85" s="1" t="s">
+        <x:v>176</x:v>
+      </x:c>
+      <x:c r="B85" s="1" t="s">
+        <x:v>177</x:v>
+      </x:c>
+      <x:c r="C85" s="1" t="s">
+        <x:v>18</x:v>
+      </x:c>
+      <x:c r="D85" s="1" t="s">
+        <x:v>6</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="86" spans="1:4" ht="13.5" customHeight="1">
+      <x:c r="A86" s="1" t="s">
+        <x:v>178</x:v>
+      </x:c>
+      <x:c r="B86" s="1" t="s">
+        <x:v>179</x:v>
+      </x:c>
+      <x:c r="C86" s="1" t="s">
+        <x:v>18</x:v>
+      </x:c>
+      <x:c r="D86" s="1" t="s">
+        <x:v>6</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="87" spans="1:4" ht="13.5" customHeight="1">
+      <x:c r="A87" s="1" t="s">
+        <x:v>180</x:v>
+      </x:c>
+      <x:c r="B87" s="1" t="s">
+        <x:v>181</x:v>
+      </x:c>
+      <x:c r="C87" s="1" t="s">
+        <x:v>86</x:v>
+      </x:c>
+      <x:c r="D87" s="1" t="s">
+        <x:v>6</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="88" spans="1:4" ht="13.5" customHeight="1">
+      <x:c r="A88" s="1" t="s">
+        <x:v>182</x:v>
+      </x:c>
+      <x:c r="B88" s="1" t="s">
+        <x:v>183</x:v>
+      </x:c>
+      <x:c r="C88" s="1" t="s">
+        <x:v>18</x:v>
+      </x:c>
+      <x:c r="D88" s="1" t="s">
+        <x:v>6</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="89" spans="1:4" ht="13.5" customHeight="1">
+      <x:c r="A89" s="1" t="s">
+        <x:v>184</x:v>
+      </x:c>
+      <x:c r="B89" s="1" t="s">
+        <x:v>185</x:v>
+      </x:c>
+      <x:c r="C89" s="1" t="s">
+        <x:v>86</x:v>
+      </x:c>
+      <x:c r="D89" s="1" t="s">
+        <x:v>6</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="90" spans="1:4" ht="13.5" customHeight="1">
+      <x:c r="A90" s="1" t="s">
+        <x:v>186</x:v>
+      </x:c>
+      <x:c r="B90" s="1" t="s">
+        <x:v>187</x:v>
+      </x:c>
+      <x:c r="C90" s="1" t="s">
+        <x:v>86</x:v>
+      </x:c>
+      <x:c r="D90" s="1" t="s">
         <x:v>6</x:v>
       </x:c>
     </x:row>

</xml_diff>

<commit_message>
More stabilisation of snippet IDs.
</commit_message>
<xml_diff>
--- a/tests/test1/output/main-loc.xlsx
+++ b/tests/test1/output/main-loc.xlsx
@@ -80,6 +80,12 @@
   </x:si>
   <x:si>
     <x:t>Glad that's over with!</x:t>
+  </x:si>
+  <x:si>
+    <x:t>main_TestScene_Q099</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Same snippet?</x:t>
   </x:si>
   <x:si>
     <x:t>main_Barks_O037</x:t>
@@ -668,8 +674,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<x:table xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:D90" totalsRowShown="0">
-  <x:autoFilter ref="A1:D90"/>
+<x:table xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:D91" totalsRowShown="0">
+  <x:autoFilter ref="A1:D91"/>
   <x:tableColumns count="4">
     <x:tableColumn id="1" name="ID" dataDxfId="0"/>
     <x:tableColumn id="2" name="Text" dataDxfId="0"/>
@@ -968,7 +974,7 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:D90"/>
+  <x:dimension ref="A1:D91"/>
   <x:sheetViews>
     <x:sheetView workbookViewId="0">
       <x:pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
@@ -1145,7 +1151,7 @@
         <x:v>31</x:v>
       </x:c>
       <x:c r="C12" s="1" t="s">
-        <x:v>32</x:v>
+        <x:v>18</x:v>
       </x:c>
       <x:c r="D12" s="1" t="s">
         <x:v>6</x:v>
@@ -1153,13 +1159,13 @@
     </x:row>
     <x:row r="13" spans="1:4" ht="13.5" customHeight="1">
       <x:c r="A13" s="1" t="s">
+        <x:v>32</x:v>
+      </x:c>
+      <x:c r="B13" s="1" t="s">
         <x:v>33</x:v>
       </x:c>
-      <x:c r="B13" s="1" t="s">
+      <x:c r="C13" s="1" t="s">
         <x:v>34</x:v>
-      </x:c>
-      <x:c r="C13" s="1" t="s">
-        <x:v>18</x:v>
       </x:c>
       <x:c r="D13" s="1" t="s">
         <x:v>6</x:v>
@@ -1201,7 +1207,7 @@
         <x:v>40</x:v>
       </x:c>
       <x:c r="C16" s="1" t="s">
-        <x:v>32</x:v>
+        <x:v>18</x:v>
       </x:c>
       <x:c r="D16" s="1" t="s">
         <x:v>6</x:v>
@@ -1215,7 +1221,7 @@
         <x:v>42</x:v>
       </x:c>
       <x:c r="C17" s="1" t="s">
-        <x:v>32</x:v>
+        <x:v>34</x:v>
       </x:c>
       <x:c r="D17" s="1" t="s">
         <x:v>6</x:v>
@@ -1226,10 +1232,10 @@
         <x:v>43</x:v>
       </x:c>
       <x:c r="B18" s="1" t="s">
-        <x:v>42</x:v>
+        <x:v>44</x:v>
       </x:c>
       <x:c r="C18" s="1" t="s">
-        <x:v>18</x:v>
+        <x:v>34</x:v>
       </x:c>
       <x:c r="D18" s="1" t="s">
         <x:v>6</x:v>
@@ -1237,10 +1243,10 @@
     </x:row>
     <x:row r="19" spans="1:4" ht="13.5" customHeight="1">
       <x:c r="A19" s="1" t="s">
+        <x:v>45</x:v>
+      </x:c>
+      <x:c r="B19" s="1" t="s">
         <x:v>44</x:v>
-      </x:c>
-      <x:c r="B19" s="1" t="s">
-        <x:v>45</x:v>
       </x:c>
       <x:c r="C19" s="1" t="s">
         <x:v>18</x:v>
@@ -1310,10 +1316,10 @@
         <x:v>54</x:v>
       </x:c>
       <x:c r="B24" s="1" t="s">
-        <x:v>42</x:v>
+        <x:v>55</x:v>
       </x:c>
       <x:c r="C24" s="1" t="s">
-        <x:v>32</x:v>
+        <x:v>18</x:v>
       </x:c>
       <x:c r="D24" s="1" t="s">
         <x:v>6</x:v>
@@ -1321,13 +1327,13 @@
     </x:row>
     <x:row r="25" spans="1:4" ht="13.5" customHeight="1">
       <x:c r="A25" s="1" t="s">
-        <x:v>55</x:v>
+        <x:v>56</x:v>
       </x:c>
       <x:c r="B25" s="1" t="s">
-        <x:v>45</x:v>
+        <x:v>44</x:v>
       </x:c>
       <x:c r="C25" s="1" t="s">
-        <x:v>32</x:v>
+        <x:v>34</x:v>
       </x:c>
       <x:c r="D25" s="1" t="s">
         <x:v>6</x:v>
@@ -1335,13 +1341,13 @@
     </x:row>
     <x:row r="26" spans="1:4" ht="13.5" customHeight="1">
       <x:c r="A26" s="1" t="s">
-        <x:v>56</x:v>
+        <x:v>57</x:v>
       </x:c>
       <x:c r="B26" s="1" t="s">
-        <x:v>57</x:v>
+        <x:v>47</x:v>
       </x:c>
       <x:c r="C26" s="1" t="s">
-        <x:v>18</x:v>
+        <x:v>34</x:v>
       </x:c>
       <x:c r="D26" s="1" t="s">
         <x:v>6</x:v>
@@ -1383,7 +1389,7 @@
         <x:v>63</x:v>
       </x:c>
       <x:c r="C29" s="1" t="s">
-        <x:v>32</x:v>
+        <x:v>18</x:v>
       </x:c>
       <x:c r="D29" s="1" t="s">
         <x:v>6</x:v>
@@ -1397,7 +1403,7 @@
         <x:v>65</x:v>
       </x:c>
       <x:c r="C30" s="1" t="s">
-        <x:v>18</x:v>
+        <x:v>34</x:v>
       </x:c>
       <x:c r="D30" s="1" t="s">
         <x:v>6</x:v>
@@ -1411,7 +1417,7 @@
         <x:v>67</x:v>
       </x:c>
       <x:c r="C31" s="1" t="s">
-        <x:v>68</x:v>
+        <x:v>18</x:v>
       </x:c>
       <x:c r="D31" s="1" t="s">
         <x:v>6</x:v>
@@ -1419,13 +1425,13 @@
     </x:row>
     <x:row r="32" spans="1:4" ht="13.5" customHeight="1">
       <x:c r="A32" s="1" t="s">
+        <x:v>68</x:v>
+      </x:c>
+      <x:c r="B32" s="1" t="s">
         <x:v>69</x:v>
       </x:c>
-      <x:c r="B32" s="1" t="s">
+      <x:c r="C32" s="1" t="s">
         <x:v>70</x:v>
-      </x:c>
-      <x:c r="C32" s="1" t="s">
-        <x:v>6</x:v>
       </x:c>
       <x:c r="D32" s="1" t="s">
         <x:v>6</x:v>
@@ -1439,7 +1445,7 @@
         <x:v>72</x:v>
       </x:c>
       <x:c r="C33" s="1" t="s">
-        <x:v>18</x:v>
+        <x:v>6</x:v>
       </x:c>
       <x:c r="D33" s="1" t="s">
         <x:v>6</x:v>
@@ -1453,7 +1459,7 @@
         <x:v>74</x:v>
       </x:c>
       <x:c r="C34" s="1" t="s">
-        <x:v>6</x:v>
+        <x:v>18</x:v>
       </x:c>
       <x:c r="D34" s="1" t="s">
         <x:v>6</x:v>
@@ -1467,7 +1473,7 @@
         <x:v>76</x:v>
       </x:c>
       <x:c r="C35" s="1" t="s">
-        <x:v>18</x:v>
+        <x:v>6</x:v>
       </x:c>
       <x:c r="D35" s="1" t="s">
         <x:v>6</x:v>
@@ -1481,7 +1487,7 @@
         <x:v>78</x:v>
       </x:c>
       <x:c r="C36" s="1" t="s">
-        <x:v>6</x:v>
+        <x:v>18</x:v>
       </x:c>
       <x:c r="D36" s="1" t="s">
         <x:v>6</x:v>
@@ -1495,7 +1501,7 @@
         <x:v>80</x:v>
       </x:c>
       <x:c r="C37" s="1" t="s">
-        <x:v>18</x:v>
+        <x:v>6</x:v>
       </x:c>
       <x:c r="D37" s="1" t="s">
         <x:v>6</x:v>
@@ -1512,49 +1518,49 @@
         <x:v>18</x:v>
       </x:c>
       <x:c r="D38" s="1" t="s">
-        <x:v>83</x:v>
+        <x:v>6</x:v>
       </x:c>
     </x:row>
     <x:row r="39" spans="1:4" ht="13.5" customHeight="1">
       <x:c r="A39" s="1" t="s">
+        <x:v>83</x:v>
+      </x:c>
+      <x:c r="B39" s="1" t="s">
         <x:v>84</x:v>
       </x:c>
-      <x:c r="B39" s="1" t="s">
+      <x:c r="C39" s="1" t="s">
+        <x:v>18</x:v>
+      </x:c>
+      <x:c r="D39" s="1" t="s">
         <x:v>85</x:v>
-      </x:c>
-      <x:c r="C39" s="1" t="s">
-        <x:v>86</x:v>
-      </x:c>
-      <x:c r="D39" s="1" t="s">
-        <x:v>6</x:v>
       </x:c>
     </x:row>
     <x:row r="40" spans="1:4" ht="13.5" customHeight="1">
       <x:c r="A40" s="1" t="s">
+        <x:v>86</x:v>
+      </x:c>
+      <x:c r="B40" s="1" t="s">
         <x:v>87</x:v>
       </x:c>
-      <x:c r="B40" s="1" t="s">
+      <x:c r="C40" s="1" t="s">
         <x:v>88</x:v>
       </x:c>
-      <x:c r="C40" s="1" t="s">
-        <x:v>18</x:v>
-      </x:c>
       <x:c r="D40" s="1" t="s">
-        <x:v>89</x:v>
+        <x:v>6</x:v>
       </x:c>
     </x:row>
     <x:row r="41" spans="1:4" ht="13.5" customHeight="1">
       <x:c r="A41" s="1" t="s">
+        <x:v>89</x:v>
+      </x:c>
+      <x:c r="B41" s="1" t="s">
         <x:v>90</x:v>
       </x:c>
-      <x:c r="B41" s="1" t="s">
+      <x:c r="C41" s="1" t="s">
+        <x:v>18</x:v>
+      </x:c>
+      <x:c r="D41" s="1" t="s">
         <x:v>91</x:v>
-      </x:c>
-      <x:c r="C41" s="1" t="s">
-        <x:v>86</x:v>
-      </x:c>
-      <x:c r="D41" s="1" t="s">
-        <x:v>6</x:v>
       </x:c>
     </x:row>
     <x:row r="42" spans="1:4" ht="13.5" customHeight="1">
@@ -1565,7 +1571,7 @@
         <x:v>93</x:v>
       </x:c>
       <x:c r="C42" s="1" t="s">
-        <x:v>86</x:v>
+        <x:v>88</x:v>
       </x:c>
       <x:c r="D42" s="1" t="s">
         <x:v>6</x:v>
@@ -1579,7 +1585,7 @@
         <x:v>95</x:v>
       </x:c>
       <x:c r="C43" s="1" t="s">
-        <x:v>86</x:v>
+        <x:v>88</x:v>
       </x:c>
       <x:c r="D43" s="1" t="s">
         <x:v>6</x:v>
@@ -1593,7 +1599,7 @@
         <x:v>97</x:v>
       </x:c>
       <x:c r="C44" s="1" t="s">
-        <x:v>6</x:v>
+        <x:v>88</x:v>
       </x:c>
       <x:c r="D44" s="1" t="s">
         <x:v>6</x:v>
@@ -1607,7 +1613,7 @@
         <x:v>99</x:v>
       </x:c>
       <x:c r="C45" s="1" t="s">
-        <x:v>68</x:v>
+        <x:v>6</x:v>
       </x:c>
       <x:c r="D45" s="1" t="s">
         <x:v>6</x:v>
@@ -1621,7 +1627,7 @@
         <x:v>101</x:v>
       </x:c>
       <x:c r="C46" s="1" t="s">
-        <x:v>32</x:v>
+        <x:v>70</x:v>
       </x:c>
       <x:c r="D46" s="1" t="s">
         <x:v>6</x:v>
@@ -1635,7 +1641,7 @@
         <x:v>103</x:v>
       </x:c>
       <x:c r="C47" s="1" t="s">
-        <x:v>6</x:v>
+        <x:v>34</x:v>
       </x:c>
       <x:c r="D47" s="1" t="s">
         <x:v>6</x:v>
@@ -1646,10 +1652,10 @@
         <x:v>104</x:v>
       </x:c>
       <x:c r="B48" s="1" t="s">
-        <x:v>103</x:v>
+        <x:v>105</x:v>
       </x:c>
       <x:c r="C48" s="1" t="s">
-        <x:v>68</x:v>
+        <x:v>6</x:v>
       </x:c>
       <x:c r="D48" s="1" t="s">
         <x:v>6</x:v>
@@ -1657,13 +1663,13 @@
     </x:row>
     <x:row r="49" spans="1:4" ht="13.5" customHeight="1">
       <x:c r="A49" s="1" t="s">
+        <x:v>106</x:v>
+      </x:c>
+      <x:c r="B49" s="1" t="s">
         <x:v>105</x:v>
       </x:c>
-      <x:c r="B49" s="1" t="s">
-        <x:v>106</x:v>
-      </x:c>
       <x:c r="C49" s="1" t="s">
-        <x:v>32</x:v>
+        <x:v>70</x:v>
       </x:c>
       <x:c r="D49" s="1" t="s">
         <x:v>6</x:v>
@@ -1677,7 +1683,7 @@
         <x:v>108</x:v>
       </x:c>
       <x:c r="C50" s="1" t="s">
-        <x:v>6</x:v>
+        <x:v>34</x:v>
       </x:c>
       <x:c r="D50" s="1" t="s">
         <x:v>6</x:v>
@@ -1688,10 +1694,10 @@
         <x:v>109</x:v>
       </x:c>
       <x:c r="B51" s="1" t="s">
-        <x:v>108</x:v>
+        <x:v>110</x:v>
       </x:c>
       <x:c r="C51" s="1" t="s">
-        <x:v>68</x:v>
+        <x:v>6</x:v>
       </x:c>
       <x:c r="D51" s="1" t="s">
         <x:v>6</x:v>
@@ -1699,13 +1705,13 @@
     </x:row>
     <x:row r="52" spans="1:4" ht="13.5" customHeight="1">
       <x:c r="A52" s="1" t="s">
+        <x:v>111</x:v>
+      </x:c>
+      <x:c r="B52" s="1" t="s">
         <x:v>110</x:v>
       </x:c>
-      <x:c r="B52" s="1" t="s">
-        <x:v>111</x:v>
-      </x:c>
       <x:c r="C52" s="1" t="s">
-        <x:v>32</x:v>
+        <x:v>70</x:v>
       </x:c>
       <x:c r="D52" s="1" t="s">
         <x:v>6</x:v>
@@ -1719,7 +1725,7 @@
         <x:v>113</x:v>
       </x:c>
       <x:c r="C53" s="1" t="s">
-        <x:v>32</x:v>
+        <x:v>34</x:v>
       </x:c>
       <x:c r="D53" s="1" t="s">
         <x:v>6</x:v>
@@ -1733,7 +1739,7 @@
         <x:v>115</x:v>
       </x:c>
       <x:c r="C54" s="1" t="s">
-        <x:v>32</x:v>
+        <x:v>34</x:v>
       </x:c>
       <x:c r="D54" s="1" t="s">
         <x:v>6</x:v>
@@ -1747,7 +1753,7 @@
         <x:v>117</x:v>
       </x:c>
       <x:c r="C55" s="1" t="s">
-        <x:v>6</x:v>
+        <x:v>34</x:v>
       </x:c>
       <x:c r="D55" s="1" t="s">
         <x:v>6</x:v>
@@ -1775,7 +1781,7 @@
         <x:v>121</x:v>
       </x:c>
       <x:c r="C57" s="1" t="s">
-        <x:v>68</x:v>
+        <x:v>6</x:v>
       </x:c>
       <x:c r="D57" s="1" t="s">
         <x:v>6</x:v>
@@ -1789,7 +1795,7 @@
         <x:v>123</x:v>
       </x:c>
       <x:c r="C58" s="1" t="s">
-        <x:v>32</x:v>
+        <x:v>70</x:v>
       </x:c>
       <x:c r="D58" s="1" t="s">
         <x:v>6</x:v>
@@ -1803,7 +1809,7 @@
         <x:v>125</x:v>
       </x:c>
       <x:c r="C59" s="1" t="s">
-        <x:v>68</x:v>
+        <x:v>34</x:v>
       </x:c>
       <x:c r="D59" s="1" t="s">
         <x:v>6</x:v>
@@ -1817,7 +1823,7 @@
         <x:v>127</x:v>
       </x:c>
       <x:c r="C60" s="1" t="s">
-        <x:v>32</x:v>
+        <x:v>70</x:v>
       </x:c>
       <x:c r="D60" s="1" t="s">
         <x:v>6</x:v>
@@ -1831,7 +1837,7 @@
         <x:v>129</x:v>
       </x:c>
       <x:c r="C61" s="1" t="s">
-        <x:v>32</x:v>
+        <x:v>34</x:v>
       </x:c>
       <x:c r="D61" s="1" t="s">
         <x:v>6</x:v>
@@ -1845,7 +1851,7 @@
         <x:v>131</x:v>
       </x:c>
       <x:c r="C62" s="1" t="s">
-        <x:v>6</x:v>
+        <x:v>34</x:v>
       </x:c>
       <x:c r="D62" s="1" t="s">
         <x:v>6</x:v>
@@ -1859,7 +1865,7 @@
         <x:v>133</x:v>
       </x:c>
       <x:c r="C63" s="1" t="s">
-        <x:v>68</x:v>
+        <x:v>6</x:v>
       </x:c>
       <x:c r="D63" s="1" t="s">
         <x:v>6</x:v>
@@ -1873,7 +1879,7 @@
         <x:v>135</x:v>
       </x:c>
       <x:c r="C64" s="1" t="s">
-        <x:v>32</x:v>
+        <x:v>70</x:v>
       </x:c>
       <x:c r="D64" s="1" t="s">
         <x:v>6</x:v>
@@ -1887,7 +1893,7 @@
         <x:v>137</x:v>
       </x:c>
       <x:c r="C65" s="1" t="s">
-        <x:v>6</x:v>
+        <x:v>34</x:v>
       </x:c>
       <x:c r="D65" s="1" t="s">
         <x:v>6</x:v>
@@ -1901,7 +1907,7 @@
         <x:v>139</x:v>
       </x:c>
       <x:c r="C66" s="1" t="s">
-        <x:v>68</x:v>
+        <x:v>6</x:v>
       </x:c>
       <x:c r="D66" s="1" t="s">
         <x:v>6</x:v>
@@ -1915,7 +1921,7 @@
         <x:v>141</x:v>
       </x:c>
       <x:c r="C67" s="1" t="s">
-        <x:v>32</x:v>
+        <x:v>70</x:v>
       </x:c>
       <x:c r="D67" s="1" t="s">
         <x:v>6</x:v>
@@ -1929,7 +1935,7 @@
         <x:v>143</x:v>
       </x:c>
       <x:c r="C68" s="1" t="s">
-        <x:v>6</x:v>
+        <x:v>34</x:v>
       </x:c>
       <x:c r="D68" s="1" t="s">
         <x:v>6</x:v>
@@ -1957,7 +1963,7 @@
         <x:v>147</x:v>
       </x:c>
       <x:c r="C70" s="1" t="s">
-        <x:v>68</x:v>
+        <x:v>6</x:v>
       </x:c>
       <x:c r="D70" s="1" t="s">
         <x:v>6</x:v>
@@ -1971,7 +1977,7 @@
         <x:v>149</x:v>
       </x:c>
       <x:c r="C71" s="1" t="s">
-        <x:v>32</x:v>
+        <x:v>70</x:v>
       </x:c>
       <x:c r="D71" s="1" t="s">
         <x:v>6</x:v>
@@ -1985,7 +1991,7 @@
         <x:v>151</x:v>
       </x:c>
       <x:c r="C72" s="1" t="s">
-        <x:v>32</x:v>
+        <x:v>34</x:v>
       </x:c>
       <x:c r="D72" s="1" t="s">
         <x:v>6</x:v>
@@ -1999,7 +2005,7 @@
         <x:v>153</x:v>
       </x:c>
       <x:c r="C73" s="1" t="s">
-        <x:v>68</x:v>
+        <x:v>34</x:v>
       </x:c>
       <x:c r="D73" s="1" t="s">
         <x:v>6</x:v>
@@ -2013,7 +2019,7 @@
         <x:v>155</x:v>
       </x:c>
       <x:c r="C74" s="1" t="s">
-        <x:v>32</x:v>
+        <x:v>70</x:v>
       </x:c>
       <x:c r="D74" s="1" t="s">
         <x:v>6</x:v>
@@ -2027,7 +2033,7 @@
         <x:v>157</x:v>
       </x:c>
       <x:c r="C75" s="1" t="s">
-        <x:v>68</x:v>
+        <x:v>34</x:v>
       </x:c>
       <x:c r="D75" s="1" t="s">
         <x:v>6</x:v>
@@ -2041,7 +2047,7 @@
         <x:v>159</x:v>
       </x:c>
       <x:c r="C76" s="1" t="s">
-        <x:v>68</x:v>
+        <x:v>70</x:v>
       </x:c>
       <x:c r="D76" s="1" t="s">
         <x:v>6</x:v>
@@ -2055,7 +2061,7 @@
         <x:v>161</x:v>
       </x:c>
       <x:c r="C77" s="1" t="s">
-        <x:v>68</x:v>
+        <x:v>70</x:v>
       </x:c>
       <x:c r="D77" s="1" t="s">
         <x:v>6</x:v>
@@ -2069,7 +2075,7 @@
         <x:v>163</x:v>
       </x:c>
       <x:c r="C78" s="1" t="s">
-        <x:v>32</x:v>
+        <x:v>70</x:v>
       </x:c>
       <x:c r="D78" s="1" t="s">
         <x:v>6</x:v>
@@ -2083,7 +2089,7 @@
         <x:v>165</x:v>
       </x:c>
       <x:c r="C79" s="1" t="s">
-        <x:v>18</x:v>
+        <x:v>34</x:v>
       </x:c>
       <x:c r="D79" s="1" t="s">
         <x:v>6</x:v>
@@ -2097,7 +2103,7 @@
         <x:v>167</x:v>
       </x:c>
       <x:c r="C80" s="1" t="s">
-        <x:v>86</x:v>
+        <x:v>18</x:v>
       </x:c>
       <x:c r="D80" s="1" t="s">
         <x:v>6</x:v>
@@ -2111,7 +2117,7 @@
         <x:v>169</x:v>
       </x:c>
       <x:c r="C81" s="1" t="s">
-        <x:v>18</x:v>
+        <x:v>88</x:v>
       </x:c>
       <x:c r="D81" s="1" t="s">
         <x:v>6</x:v>
@@ -2195,7 +2201,7 @@
         <x:v>181</x:v>
       </x:c>
       <x:c r="C87" s="1" t="s">
-        <x:v>86</x:v>
+        <x:v>18</x:v>
       </x:c>
       <x:c r="D87" s="1" t="s">
         <x:v>6</x:v>
@@ -2209,7 +2215,7 @@
         <x:v>183</x:v>
       </x:c>
       <x:c r="C88" s="1" t="s">
-        <x:v>18</x:v>
+        <x:v>88</x:v>
       </x:c>
       <x:c r="D88" s="1" t="s">
         <x:v>6</x:v>
@@ -2223,7 +2229,7 @@
         <x:v>185</x:v>
       </x:c>
       <x:c r="C89" s="1" t="s">
-        <x:v>86</x:v>
+        <x:v>18</x:v>
       </x:c>
       <x:c r="D89" s="1" t="s">
         <x:v>6</x:v>
@@ -2237,9 +2243,23 @@
         <x:v>187</x:v>
       </x:c>
       <x:c r="C90" s="1" t="s">
-        <x:v>86</x:v>
+        <x:v>88</x:v>
       </x:c>
       <x:c r="D90" s="1" t="s">
+        <x:v>6</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="91" spans="1:4" ht="13.5" customHeight="1">
+      <x:c r="A91" s="1" t="s">
+        <x:v>188</x:v>
+      </x:c>
+      <x:c r="B91" s="1" t="s">
+        <x:v>189</x:v>
+      </x:c>
+      <x:c r="C91" s="1" t="s">
+        <x:v>88</x:v>
+      </x:c>
+      <x:c r="D91" s="1" t="s">
         <x:v>6</x:v>
       </x:c>
     </x:row>

</xml_diff>

<commit_message>
More stability - use LineIDs for Jaccard comparison
</commit_message>
<xml_diff>
--- a/tests/test1/output/main-loc.xlsx
+++ b/tests/test1/output/main-loc.xlsx
@@ -151,13 +151,13 @@
     <x:t>This is a line.</x:t>
   </x:si>
   <x:si>
+    <x:t>main_Recording_PartB_1RQS</x:t>
+  </x:si>
+  <x:si>
+    <x:t>This is also a line.</x:t>
+  </x:si>
+  <x:si>
     <x:t>main_Recording_PartB_FH4U</x:t>
-  </x:si>
-  <x:si>
-    <x:t>main_Recording_PartB_1RQS</x:t>
-  </x:si>
-  <x:si>
-    <x:t>This is also a line.</x:t>
   </x:si>
   <x:si>
     <x:t>main_Recording_PartC_JITN</x:t>
@@ -1246,7 +1246,7 @@
         <x:v>45</x:v>
       </x:c>
       <x:c r="B19" s="1" t="s">
-        <x:v>44</x:v>
+        <x:v>46</x:v>
       </x:c>
       <x:c r="C19" s="1" t="s">
         <x:v>18</x:v>
@@ -1257,10 +1257,10 @@
     </x:row>
     <x:row r="20" spans="1:4" ht="13.5" customHeight="1">
       <x:c r="A20" s="1" t="s">
-        <x:v>46</x:v>
+        <x:v>47</x:v>
       </x:c>
       <x:c r="B20" s="1" t="s">
-        <x:v>47</x:v>
+        <x:v>44</x:v>
       </x:c>
       <x:c r="C20" s="1" t="s">
         <x:v>18</x:v>
@@ -1344,7 +1344,7 @@
         <x:v>57</x:v>
       </x:c>
       <x:c r="B26" s="1" t="s">
-        <x:v>47</x:v>
+        <x:v>46</x:v>
       </x:c>
       <x:c r="C26" s="1" t="s">
         <x:v>34</x:v>

</xml_diff>